<commit_message>
type tir pour la fronde
</commit_message>
<xml_diff>
--- a/outils/armes.xlsx
+++ b/outils/armes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E42FAC-02D3-4473-91A2-30B9F6C8CF46}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="111">
   <si>
     <t>Nom</t>
   </si>
@@ -358,12 +359,15 @@
   </si>
   <si>
     <t>3D12</t>
+  </si>
+  <si>
+    <t>Tir(1, 0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -598,6 +602,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -610,10 +618,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -893,11 +897,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AA35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,22 +925,22 @@
       <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30" t="s">
+      <c r="D2" s="32"/>
+      <c r="E2" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30" t="s">
+      <c r="H2" s="32"/>
+      <c r="I2" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="30"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="10" t="s">
         <v>1</v>
       </c>
@@ -968,7 +972,7 @@
       <c r="U2" s="10"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
+      <c r="A3" s="29"/>
       <c r="B3" s="11" t="s">
         <v>10</v>
       </c>
@@ -1015,19 +1019,19 @@
       </c>
       <c r="R3" s="17"/>
       <c r="S3" s="18"/>
-      <c r="T3" s="31" t="str">
+      <c r="T3" s="27" t="str">
         <f>CONCATENATE("&lt;tr&gt;&lt;td&gt;", B3, "&lt;/td&gt;&lt;td class=""rapide""&gt;",C3,"+",D3,"&lt;/td&gt;&lt;td class=""precis""&gt;",E3,"+",F3,"&lt;/td&gt;&lt;td class=""puissant""&gt;",G3,"+",H3,"&lt;/td&gt;&lt;td class=""distance""&gt;",I3,"+",J3,"&lt;/td&gt;&lt;td class=""parade""&gt;",O3,"&lt;/td&gt;&lt;td&gt;",P3,"&lt;/td&gt;&lt;td&gt;",Q3,"&lt;/td&gt;&lt;td&gt;",R3,"&lt;/td&gt;&lt;td&gt;",S3,"&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;tr&gt;&lt;td&gt;Couteau&lt;/td&gt;&lt;td class="rapide"&gt;2D4+&lt;/td&gt;&lt;td class="precis"&gt;2D4+&lt;/td&gt;&lt;td class="puissant"&gt;1D4+&lt;/td&gt;&lt;td class="distance"&gt;3D4+&lt;/td&gt;&lt;td class="parade"&gt;-2&lt;/td&gt;&lt;td&gt;0.5kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U3" s="31"/>
-      <c r="Y3" s="28" t="s">
+      <c r="U3" s="27"/>
+      <c r="Y3" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="Z3" s="28"/>
-      <c r="AA3" s="28"/>
+      <c r="Z3" s="30"/>
+      <c r="AA3" s="30"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="11" t="s">
         <v>15</v>
       </c>
@@ -1074,11 +1078,11 @@
       </c>
       <c r="R4" s="17"/>
       <c r="S4" s="18"/>
-      <c r="T4" s="31" t="str">
+      <c r="T4" s="27" t="str">
         <f t="shared" ref="T4:T35" si="0">CONCATENATE("&lt;tr&gt;&lt;td&gt;", B4, "&lt;/td&gt;&lt;td class=""rapide""&gt;",C4,"+",D4,"&lt;/td&gt;&lt;td class=""precis""&gt;",E4,"+",F4,"&lt;/td&gt;&lt;td class=""puissant""&gt;",G4,"+",H4,"&lt;/td&gt;&lt;td class=""distance""&gt;",I4,"+",J4,"&lt;/td&gt;&lt;td class=""parade""&gt;",O4,"&lt;/td&gt;&lt;td&gt;",P4,"&lt;/td&gt;&lt;td&gt;",Q4,"&lt;/td&gt;&lt;td&gt;",R4,"&lt;/td&gt;&lt;td&gt;",S4,"&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;tr&gt;&lt;td&gt;Dague&lt;/td&gt;&lt;td class="rapide"&gt;3D4+&lt;/td&gt;&lt;td class="precis"&gt;2D4+&lt;/td&gt;&lt;td class="puissant"&gt;1D4+&lt;/td&gt;&lt;td class="distance"&gt;2D4+&lt;/td&gt;&lt;td class="parade"&gt;0&lt;/td&gt;&lt;td&gt;0.5kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U4" s="31"/>
+      <c r="U4" s="27"/>
       <c r="Y4" s="26" t="s">
         <v>87</v>
       </c>
@@ -1090,7 +1094,7 @@
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
@@ -1139,11 +1143,11 @@
       </c>
       <c r="R5" s="17"/>
       <c r="S5" s="18"/>
-      <c r="T5" s="31" t="str">
+      <c r="T5" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Epée courte&lt;/td&gt;&lt;td class="rapide"&gt;3D4+&lt;/td&gt;&lt;td class="precis"&gt;2D4+&lt;/td&gt;&lt;td class="puissant"&gt;2D4+2&lt;/td&gt;&lt;td class="distance"&gt;1D4+&lt;/td&gt;&lt;td class="parade"&gt;2&lt;/td&gt;&lt;td&gt;1kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U5" s="31"/>
+      <c r="U5" s="27"/>
       <c r="X5" s="6" t="s">
         <v>69</v>
       </c>
@@ -1158,7 +1162,7 @@
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="11" t="s">
         <v>20</v>
       </c>
@@ -1209,11 +1213,11 @@
       </c>
       <c r="R6" s="17"/>
       <c r="S6" s="18"/>
-      <c r="T6" s="31" t="str">
+      <c r="T6" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Hachette&lt;/td&gt;&lt;td class="rapide"&gt;3D4+2&lt;/td&gt;&lt;td class="precis"&gt;1D4+&lt;/td&gt;&lt;td class="puissant"&gt;1D4+&lt;/td&gt;&lt;td class="distance"&gt;3D4+2&lt;/td&gt;&lt;td class="parade"&gt;-4&lt;/td&gt;&lt;td&gt;1kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U6" s="31"/>
+      <c r="U6" s="27"/>
       <c r="X6" s="7" t="s">
         <v>71</v>
       </c>
@@ -1228,7 +1232,7 @@
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="11" t="s">
         <v>31</v>
       </c>
@@ -1275,11 +1279,11 @@
       </c>
       <c r="R7" s="17"/>
       <c r="S7" s="18"/>
-      <c r="T7" s="31" t="str">
+      <c r="T7" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Rondache&lt;/td&gt;&lt;td class="rapide"&gt;1D4+&lt;/td&gt;&lt;td class="precis"&gt;1D4+&lt;/td&gt;&lt;td class="puissant"&gt;1D4+&lt;/td&gt;&lt;td class="distance"&gt;1D4+&lt;/td&gt;&lt;td class="parade"&gt;4&lt;/td&gt;&lt;td&gt;2kg&lt;/td&gt;&lt;td&gt;0&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U7" s="31"/>
+      <c r="U7" s="27"/>
       <c r="X7" s="8" t="s">
         <v>70</v>
       </c>
@@ -1294,7 +1298,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="11" t="s">
         <v>68</v>
       </c>
@@ -1337,12 +1341,14 @@
         <v>2</v>
       </c>
       <c r="R8" s="17"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="31" t="str">
+      <c r="S8" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="T8" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;Fronde&lt;/td&gt;&lt;td class="rapide"&gt;1D4+&lt;/td&gt;&lt;td class="precis"&gt;1D4+&lt;/td&gt;&lt;td class="puissant"&gt;1D4+&lt;/td&gt;&lt;td class="distance"&gt;4D4+&lt;/td&gt;&lt;td class="parade"&gt;-4&lt;/td&gt;&lt;td&gt;0.5kg&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
-      </c>
-      <c r="U8" s="31"/>
+        <v>&lt;tr&gt;&lt;td&gt;Fronde&lt;/td&gt;&lt;td class="rapide"&gt;1D4+&lt;/td&gt;&lt;td class="precis"&gt;1D4+&lt;/td&gt;&lt;td class="puissant"&gt;1D4+&lt;/td&gt;&lt;td class="distance"&gt;4D4+&lt;/td&gt;&lt;td class="parade"&gt;-4&lt;/td&gt;&lt;td&gt;0.5kg&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td&gt;Tir(1, 0)&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="U8" s="27"/>
       <c r="X8" s="1" t="s">
         <v>72</v>
       </c>
@@ -1357,7 +1363,7 @@
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="11" t="s">
         <v>38</v>
       </c>
@@ -1406,14 +1412,14 @@
       </c>
       <c r="R9" s="17"/>
       <c r="S9" s="18"/>
-      <c r="T9" s="31" t="str">
+      <c r="T9" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Masse&lt;/td&gt;&lt;td class="rapide"&gt;1D4+&lt;/td&gt;&lt;td class="precis"&gt;2D4+&lt;/td&gt;&lt;td class="puissant"&gt;3D4+2&lt;/td&gt;&lt;td class="distance"&gt;1D4+&lt;/td&gt;&lt;td class="parade"&gt;0&lt;/td&gt;&lt;td&gt;2kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U9" s="31"/>
+      <c r="U9" s="27"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="11" t="s">
         <v>46</v>
       </c>
@@ -1466,19 +1472,19 @@
       </c>
       <c r="R10" s="17"/>
       <c r="S10" s="18"/>
-      <c r="T10" s="31" t="str">
+      <c r="T10" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Bâton&lt;/td&gt;&lt;td class="rapide"&gt;2D4+2&lt;/td&gt;&lt;td class="precis"&gt;2D4+2&lt;/td&gt;&lt;td class="puissant"&gt;2D4+4&lt;/td&gt;&lt;td class="distance"&gt;1D4+&lt;/td&gt;&lt;td class="parade"&gt;2&lt;/td&gt;&lt;td&gt;2kg&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U10" s="31"/>
+      <c r="U10" s="27"/>
       <c r="X10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="Y10" s="29" t="s">
+      <c r="Y10" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="Z10" s="29"/>
-      <c r="AA10" s="29"/>
+      <c r="Z10" s="31"/>
+      <c r="AA10" s="31"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B12" s="21" t="s">
@@ -1529,19 +1535,19 @@
         <v>102</v>
       </c>
       <c r="S12" s="18"/>
-      <c r="T12" s="31" t="str">
+      <c r="T12" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Sabre&lt;/td&gt;&lt;td class="rapide"&gt;3D8+&lt;/td&gt;&lt;td class="precis"&gt;2D8+&lt;/td&gt;&lt;td class="puissant"&gt;1D6+&lt;/td&gt;&lt;td class="distance"&gt;1D6+&lt;/td&gt;&lt;td class="parade"&gt;0&lt;/td&gt;&lt;td&gt;1kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;15 Vivacité&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U12" s="31"/>
+      <c r="U12" s="27"/>
       <c r="X12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Y12" s="29" t="s">
+      <c r="Y12" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="Z12" s="29"/>
-      <c r="AA12" s="29"/>
+      <c r="Z12" s="31"/>
+      <c r="AA12" s="31"/>
     </row>
     <row r="13" spans="1:27" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B13" s="21" t="s">
@@ -1595,12 +1601,12 @@
       <c r="S13" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="T13" s="31" t="str">
+      <c r="T13" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Arc court&lt;/td&gt;&lt;td class="rapide"&gt;1D4+&lt;/td&gt;&lt;td class="precis"&gt;1D4+&lt;/td&gt;&lt;td class="puissant"&gt;1D4+&lt;/td&gt;&lt;td class="distance"&gt;4D8+2&lt;/td&gt;&lt;td class="parade"&gt;-4&lt;/td&gt;&lt;td&gt;1kg&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;td&gt;8 Vigueur
 8 Adresse&lt;/td&gt;&lt;td&gt;Perforant, Tir(3, 0), Projectile&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U13" s="31"/>
+      <c r="U13" s="27"/>
       <c r="X13" s="2" t="s">
         <v>93</v>
       </c>
@@ -1651,11 +1657,11 @@
         <v>108</v>
       </c>
       <c r="S14" s="18"/>
-      <c r="T14" s="31" t="str">
+      <c r="T14" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Glaive&lt;/td&gt;&lt;td class="rapide"&gt;2D8+&lt;/td&gt;&lt;td class="precis"&gt;2D8+&lt;/td&gt;&lt;td class="puissant"&gt;2D8+2&lt;/td&gt;&lt;td class="distance"&gt;1D6+&lt;/td&gt;&lt;td class="parade"&gt;2&lt;/td&gt;&lt;td&gt;1kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;12 Vivacité&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U14" s="31"/>
+      <c r="U14" s="27"/>
       <c r="X14" s="2" t="s">
         <v>80</v>
       </c>
@@ -1708,11 +1714,11 @@
         <v>96</v>
       </c>
       <c r="S15" s="18"/>
-      <c r="T15" s="31" t="str">
+      <c r="T15" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Francisque&lt;/td&gt;&lt;td class="rapide"&gt;1D6+&lt;/td&gt;&lt;td class="precis"&gt;1D6+&lt;/td&gt;&lt;td class="puissant"&gt;2D8+4&lt;/td&gt;&lt;td class="distance"&gt;3D8+2&lt;/td&gt;&lt;td class="parade"&gt;-4&lt;/td&gt;&lt;td&gt;1.5kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;15 Adresse&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U15" s="31"/>
+      <c r="U15" s="27"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B16" s="21" t="s">
@@ -1765,11 +1771,11 @@
       <c r="S16" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="T16" s="31" t="str">
+      <c r="T16" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Javeline&lt;/td&gt;&lt;td class="rapide"&gt;2D8+&lt;/td&gt;&lt;td class="precis"&gt;1D6+&lt;/td&gt;&lt;td class="puissant"&gt;1D6+&lt;/td&gt;&lt;td class="distance"&gt;3D8+&lt;/td&gt;&lt;td class="parade"&gt;0&lt;/td&gt;&lt;td&gt;1kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;15 Adresse&lt;/td&gt;&lt;td&gt;Perforant&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U16" s="31"/>
+      <c r="U16" s="27"/>
     </row>
     <row r="17" spans="2:21" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
@@ -1822,12 +1828,12 @@
         <v>61</v>
       </c>
       <c r="S17" s="18"/>
-      <c r="T17" s="31" t="str">
+      <c r="T17" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Epée longue&lt;/td&gt;&lt;td class="rapide"&gt;1D6+&lt;/td&gt;&lt;td class="precis"&gt;3D8+&lt;/td&gt;&lt;td class="puissant"&gt;2D8+2&lt;/td&gt;&lt;td class="distance"&gt;1D4+&lt;/td&gt;&lt;td class="parade"&gt;2&lt;/td&gt;&lt;td&gt;1.5kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;10 Vigueur
 10 Adresse&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U17" s="31"/>
+      <c r="U17" s="27"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
@@ -1880,11 +1886,11 @@
         <v>103</v>
       </c>
       <c r="S18" s="18"/>
-      <c r="T18" s="31" t="str">
+      <c r="T18" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Hache de guerre&lt;/td&gt;&lt;td class="rapide"&gt;1D6+&lt;/td&gt;&lt;td class="precis"&gt;1D6+&lt;/td&gt;&lt;td class="puissant"&gt;3D8+4&lt;/td&gt;&lt;td class="distance"&gt;1D4+&lt;/td&gt;&lt;td class="parade"&gt;-4&lt;/td&gt;&lt;td&gt;2kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;15 Vigueur&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U18" s="31"/>
+      <c r="U18" s="27"/>
     </row>
     <row r="19" spans="2:21" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="21" t="s">
@@ -1938,12 +1944,12 @@
       <c r="S19" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="T19" s="31" t="str">
+      <c r="T19" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Arc long&lt;/td&gt;&lt;td class="rapide"&gt;1D4+&lt;/td&gt;&lt;td class="precis"&gt;1D4+&lt;/td&gt;&lt;td class="puissant"&gt;1D4+&lt;/td&gt;&lt;td class="distance"&gt;4D10+4&lt;/td&gt;&lt;td class="parade"&gt;-4&lt;/td&gt;&lt;td&gt;2kg&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;td&gt;12 Vigueur
 12 Adresse&lt;/td&gt;&lt;td&gt;Tir(4, 2), Perforant, Projectile&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U19" s="31"/>
+      <c r="U19" s="27"/>
     </row>
     <row r="20" spans="2:21" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B20" s="21" t="s">
@@ -2000,12 +2006,12 @@
       <c r="S20" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="T20" s="31" t="str">
+      <c r="T20" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Lance&lt;/td&gt;&lt;td class="rapide"&gt;1D6+&lt;/td&gt;&lt;td class="precis"&gt;3D8+2&lt;/td&gt;&lt;td class="puissant"&gt;2D8+4&lt;/td&gt;&lt;td class="distance"&gt;1D6+&lt;/td&gt;&lt;td class="parade"&gt;0&lt;/td&gt;&lt;td&gt;3kg&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;td&gt;12 Vigueur
 10 Adresse&lt;/td&gt;&lt;td&gt;Arme d’hast&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U20" s="31"/>
+      <c r="U20" s="27"/>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" s="21" t="s">
@@ -2056,11 +2062,11 @@
         <v>103</v>
       </c>
       <c r="S21" s="18"/>
-      <c r="T21" s="31" t="str">
+      <c r="T21" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Ecu&lt;/td&gt;&lt;td class="rapide"&gt;1D4+&lt;/td&gt;&lt;td class="precis"&gt;1D4+&lt;/td&gt;&lt;td class="puissant"&gt;1D4+&lt;/td&gt;&lt;td class="distance"&gt;1D4+&lt;/td&gt;&lt;td class="parade"&gt;6&lt;/td&gt;&lt;td&gt;3kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;15 Vigueur&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U21" s="31"/>
+      <c r="U21" s="27"/>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" s="21" t="s">
@@ -2113,11 +2119,11 @@
         <v>103</v>
       </c>
       <c r="S22" s="18"/>
-      <c r="T22" s="31" t="str">
+      <c r="T22" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Marteau&lt;/td&gt;&lt;td class="rapide"&gt;1D6+&lt;/td&gt;&lt;td class="precis"&gt;2D8+&lt;/td&gt;&lt;td class="puissant"&gt;3D8+2&lt;/td&gt;&lt;td class="distance"&gt;1D4+&lt;/td&gt;&lt;td class="parade"&gt;0&lt;/td&gt;&lt;td&gt;4kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;15 Vigueur&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U22" s="31"/>
+      <c r="U22" s="27"/>
     </row>
     <row r="23" spans="2:21" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B23" s="21" t="s">
@@ -2172,12 +2178,12 @@
         <v>98</v>
       </c>
       <c r="S23" s="18"/>
-      <c r="T23" s="31" t="str">
+      <c r="T23" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Epée à deux mains&lt;/td&gt;&lt;td class="rapide"&gt;1D6+&lt;/td&gt;&lt;td class="precis"&gt;2D8+2&lt;/td&gt;&lt;td class="puissant"&gt;3D8+4&lt;/td&gt;&lt;td class="distance"&gt;1D4+&lt;/td&gt;&lt;td class="parade"&gt;0&lt;/td&gt;&lt;td&gt;2kg&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;td&gt;12 Vigueur
 12 Adresse&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U23" s="31"/>
+      <c r="U23" s="27"/>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B25" s="24" t="s">
@@ -2222,11 +2228,11 @@
         <v>101</v>
       </c>
       <c r="S25" s="18"/>
-      <c r="T25" s="31" t="str">
+      <c r="T25" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Griffe&lt;/td&gt;&lt;td class="rapide"&gt;3D12+2&lt;/td&gt;&lt;td class="precis"&gt;1D6+&lt;/td&gt;&lt;td class="puissant"&gt;1D6+&lt;/td&gt;&lt;td class="distance"&gt;1D4+&lt;/td&gt;&lt;td class="parade"&gt;2&lt;/td&gt;&lt;td&gt;0.5kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;20 Vivacité&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U25" s="31"/>
+      <c r="U25" s="27"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B26" s="24" t="s">
@@ -2271,11 +2277,11 @@
       <c r="S26" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="T26" s="31" t="str">
+      <c r="T26" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Rapière&lt;/td&gt;&lt;td class="rapide"&gt;2D10+&lt;/td&gt;&lt;td class="precis"&gt;3D12+&lt;/td&gt;&lt;td class="puissant"&gt;1D6+&lt;/td&gt;&lt;td class="distance"&gt;1D6+&lt;/td&gt;&lt;td class="parade"&gt;2&lt;/td&gt;&lt;td&gt;1kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;20 Vivacité&lt;/td&gt;&lt;td&gt;Perforant&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U26" s="31"/>
+      <c r="U26" s="27"/>
     </row>
     <row r="27" spans="2:21" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B27" s="24" t="s">
@@ -2327,12 +2333,12 @@
       <c r="S27" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="T27" s="31" t="str">
+      <c r="T27" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Arbalète de poing&lt;/td&gt;&lt;td class="rapide"&gt;1D4+&lt;/td&gt;&lt;td class="precis"&gt;1D4+&lt;/td&gt;&lt;td class="puissant"&gt;1D4+&lt;/td&gt;&lt;td class="distance"&gt;4D8+&lt;/td&gt;&lt;td class="parade"&gt;-4&lt;/td&gt;&lt;td&gt;1kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;18 Vigueur
 15 Adresse&lt;/td&gt;&lt;td&gt;Perforant, Tir(2, 7), Projectile&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U27" s="31"/>
+      <c r="U27" s="27"/>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B28" s="24" t="s">
@@ -2377,11 +2383,11 @@
         <v>99</v>
       </c>
       <c r="S28" s="18"/>
-      <c r="T28" s="31" t="str">
+      <c r="T28" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Fléau d'arme&lt;/td&gt;&lt;td class="rapide"&gt;2D10+&lt;/td&gt;&lt;td class="precis"&gt;1D6+&lt;/td&gt;&lt;td class="puissant"&gt;3D12+2&lt;/td&gt;&lt;td class="distance"&gt;1D4+&lt;/td&gt;&lt;td class="parade"&gt;-4&lt;/td&gt;&lt;td&gt;2.5kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;20 Vigueur&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U28" s="31"/>
+      <c r="U28" s="27"/>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B29" s="24" t="s">
@@ -2436,11 +2442,11 @@
         <v>99</v>
       </c>
       <c r="S29" s="18"/>
-      <c r="T29" s="31" t="str">
+      <c r="T29" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Masse de guerre&lt;/td&gt;&lt;td class="rapide"&gt;1D6+&lt;/td&gt;&lt;td class="precis"&gt;2D10+2&lt;/td&gt;&lt;td class="puissant"&gt;3D12+4&lt;/td&gt;&lt;td class="distance"&gt;1D4+&lt;/td&gt;&lt;td class="parade"&gt;0&lt;/td&gt;&lt;td&gt;5kg&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;td&gt;20 Vigueur&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U29" s="31"/>
+      <c r="U29" s="27"/>
     </row>
     <row r="30" spans="2:21" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B30" s="24" t="s">
@@ -2487,12 +2493,12 @@
         <v>105</v>
       </c>
       <c r="S30" s="18"/>
-      <c r="T30" s="31" t="str">
+      <c r="T30" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Claymore&lt;/td&gt;&lt;td class="rapide"&gt;1D6+&lt;/td&gt;&lt;td class="precis"&gt;2D10+2&lt;/td&gt;&lt;td class="puissant"&gt;3D12+4&lt;/td&gt;&lt;td class="distance"&gt;1D4+&lt;/td&gt;&lt;td class="parade"&gt;0&lt;/td&gt;&lt;td&gt;3kg&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;td&gt;18 Vigueur
 18 Adresse&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U30" s="31"/>
+      <c r="U30" s="27"/>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B31" s="24" t="s">
@@ -2545,11 +2551,11 @@
         <v>99</v>
       </c>
       <c r="S31" s="18"/>
-      <c r="T31" s="31" t="str">
+      <c r="T31" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Hache de bataille&lt;/td&gt;&lt;td class="rapide"&gt;1D6+&lt;/td&gt;&lt;td class="precis"&gt;1D6+&lt;/td&gt;&lt;td class="puissant"&gt;3D12+6&lt;/td&gt;&lt;td class="distance"&gt;1D6+&lt;/td&gt;&lt;td class="parade"&gt;-4&lt;/td&gt;&lt;td&gt;3kg&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;td&gt;20 Vigueur&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U31" s="31"/>
+      <c r="U31" s="27"/>
     </row>
     <row r="32" spans="2:21" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B32" s="24" t="s">
@@ -2603,12 +2609,12 @@
       <c r="S32" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="T32" s="31" t="str">
+      <c r="T32" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Arbalète&lt;/td&gt;&lt;td class="rapide"&gt;1D4+&lt;/td&gt;&lt;td class="precis"&gt;1D4+&lt;/td&gt;&lt;td class="puissant"&gt;1D4+&lt;/td&gt;&lt;td class="distance"&gt;4D12+4&lt;/td&gt;&lt;td class="parade"&gt;-4&lt;/td&gt;&lt;td&gt;3kg&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;td&gt;20 Vigueur
 18 Adresse&lt;/td&gt;&lt;td&gt;Tir(5, 5), Perforant, Projectile&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U32" s="31"/>
+      <c r="U32" s="27"/>
     </row>
     <row r="33" spans="2:21" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B33" s="24" t="s">
@@ -2665,12 +2671,12 @@
       <c r="S33" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="T33" s="31" t="str">
+      <c r="T33" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Pique&lt;/td&gt;&lt;td class="rapide"&gt;1D6+&lt;/td&gt;&lt;td class="precis"&gt;3D12+2&lt;/td&gt;&lt;td class="puissant"&gt;2D10+2&lt;/td&gt;&lt;td class="distance"&gt;1D4+&lt;/td&gt;&lt;td class="parade"&gt;0&lt;/td&gt;&lt;td&gt;5kg&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;td&gt;18 Adresse
 15 Vigueur&lt;/td&gt;&lt;td&gt;Arme d’hast&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U33" s="31"/>
+      <c r="U33" s="27"/>
     </row>
     <row r="34" spans="2:21" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B34" s="24" t="s">
@@ -2717,12 +2723,12 @@
       <c r="S34" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="T34" s="31" t="str">
+      <c r="T34" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Hallebarde&lt;/td&gt;&lt;td class="rapide"&gt;1D6+&lt;/td&gt;&lt;td class="precis"&gt;2D10+&lt;/td&gt;&lt;td class="puissant"&gt;3D12+4&lt;/td&gt;&lt;td class="distance"&gt;1D4+&lt;/td&gt;&lt;td class="parade"&gt;0&lt;/td&gt;&lt;td&gt;5kg&lt;/td&gt;&lt;td&gt;2&lt;/td&gt;&lt;td&gt;18 Vigueur
 15 Adresse&lt;/td&gt;&lt;td&gt;Arme d’hast&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U34" s="31"/>
+      <c r="U34" s="27"/>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B35" s="24" t="s">
@@ -2773,11 +2779,11 @@
         <v>99</v>
       </c>
       <c r="S35" s="25"/>
-      <c r="T35" s="31" t="str">
+      <c r="T35" s="27" t="str">
         <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;Pavois&lt;/td&gt;&lt;td class="rapide"&gt;1D4+&lt;/td&gt;&lt;td class="precis"&gt;1D4+&lt;/td&gt;&lt;td class="puissant"&gt;1D4+&lt;/td&gt;&lt;td class="distance"&gt;1D4+&lt;/td&gt;&lt;td class="parade"&gt;10&lt;/td&gt;&lt;td&gt;5kg&lt;/td&gt;&lt;td&gt;1&lt;/td&gt;&lt;td&gt;20 Vigueur&lt;/td&gt;&lt;td&gt;&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="U35" s="32"/>
+      <c r="U35" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>